<commit_message>
v0.45beta hover light buttons
</commit_message>
<xml_diff>
--- a/структура.xlsx
+++ b/структура.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Tasks (таблица задач для каждого проекта id)</t>
   </si>
@@ -58,6 +58,18 @@
   </si>
   <si>
     <t>PROJECTS (список проектов)</t>
+  </si>
+  <si>
+    <t>payment TEXT</t>
+  </si>
+  <si>
+    <t>free</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>wait</t>
   </si>
 </sst>
 </file>
@@ -81,7 +93,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -198,6 +210,17 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -205,6 +228,30 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -213,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -221,14 +268,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -530,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,116 +591,135 @@
     <col min="1" max="1" width="10.28515625" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
     <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
-    <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="22" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" customWidth="1"/>
-    <col min="11" max="11" width="22" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="4" max="5" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="22" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" customWidth="1"/>
+    <col min="12" max="12" width="22" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="E2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="H2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="J2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="K2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="M2" s="14" t="s">
         <v>6</v>
       </c>
+      <c r="N2" s="15" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="11">
         <v>37561</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="11">
         <v>38657</v>
       </c>
-      <c r="F3" s="1">
+      <c r="E3" s="17"/>
+      <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="3"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="11">
         <v>37561</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="11">
         <v>40483</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="2"/>
+      <c r="E4" s="17"/>
+      <c r="G4" s="1"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="3"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
-      <c r="D5" s="6"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
+      <c r="G5" s="4"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
-      <c r="L5" s="6"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
v0.5beta bay buttons add
</commit_message>
<xml_diff>
--- a/структура.xlsx
+++ b/структура.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Tasks (таблица задач для каждого проекта id)</t>
   </si>
@@ -260,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -278,7 +278,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -583,7 +582,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,7 +662,9 @@
       <c r="D3" s="11">
         <v>38657</v>
       </c>
-      <c r="E3" s="17"/>
+      <c r="E3" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G3" s="1">
         <v>1</v>
       </c>
@@ -692,7 +693,9 @@
       <c r="D4" s="11">
         <v>40483</v>
       </c>
-      <c r="E4" s="17"/>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -709,7 +712,9 @@
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
+      <c r="E5" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="G5" s="4"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>

</xml_diff>

<commit_message>
v0.6beta save option add
</commit_message>
<xml_diff>
--- a/структура.xlsx
+++ b/структура.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>Tasks (таблица задач для каждого проекта id)</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>wait</t>
+  </si>
+  <si>
+    <t>OPTIONS</t>
+  </si>
+  <si>
+    <t>window_geometry TEXT</t>
+  </si>
+  <si>
+    <t>complete_visible BOOLEAN</t>
+  </si>
+  <si>
+    <t>current_visible BOOLEAN</t>
   </si>
 </sst>
 </file>
@@ -93,7 +105,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -256,11 +268,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -278,6 +303,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -579,18 +607,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="5" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
     <col min="10" max="10" width="22" customWidth="1"/>
@@ -725,6 +754,47 @@
       <c r="N5" s="6" t="s">
         <v>17</v>
       </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="18"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>